<commit_message>
Worked on the effects doc. + Cleaned the GrimReaper skills doc.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/_Done/6-GrimReaper/Documentation/GrimReaperSkills.xlsx
+++ b/GameDesign/Class/_Done/6-GrimReaper/Documentation/GrimReaperSkills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="1-ProtectiveWings" sheetId="1" r:id="rId1"/>
@@ -33,16 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="90">
-  <si>
-    <t>[[Number of casts per turn: - ]]</t>
-  </si>
-  <si>
-    <t>[[Number of cast per turn per target: - ]]</t>
-  </si>
-  <si>
-    <t>[[Max effect accumulation: - ]]</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="83">
   <si>
     <t>Additional Info</t>
   </si>
@@ -65,27 +56,15 @@
     <t>[[Number of turns between two casts: 6 ]]</t>
   </si>
   <si>
-    <t>[[Max effect accumulation: 1 ]]</t>
-  </si>
-  <si>
     <t>[[Area of effect: - Single cell]]</t>
   </si>
   <si>
-    <t>[[Invulnerable]] (1 turn)</t>
-  </si>
-  <si>
-    <t>[[Unmovable]]   (1 turn)</t>
-  </si>
-  <si>
     <t>Automatically end turn.</t>
   </si>
   <si>
     <t>Black Mist</t>
   </si>
   <si>
-    <t>[[Reduce range by 100]] (2 turns)</t>
-  </si>
-  <si>
     <t>[[AP: 5 ]]</t>
   </si>
   <si>
@@ -95,9 +74,6 @@
     <t>[[Number of turns between two casts: 7 ]]</t>
   </si>
   <si>
-    <t>Every entity except the caster loose all the range.</t>
-  </si>
-  <si>
     <t>[[Area of effect: - Every entity except the caster ]]</t>
   </si>
   <si>
@@ -143,27 +119,9 @@
     <t>[[Number of turns between two casts: 2 ]]</t>
   </si>
   <si>
-    <t>Effect name: ''Reanimated''.</t>
-  </si>
-  <si>
-    <t>Effect name: ''Zombification''.</t>
-  </si>
-  <si>
-    <t>Target: Reanimate whit the ''Zombification'' effect. (00 turns)</t>
-  </si>
-  <si>
     <t>Reanimate an K/O entity.                                                                      Can't be reanimated a second time.                                                               The reanimated entity take damage from healing but get healed from poison.                                                                                      The target must be K/O.</t>
   </si>
   <si>
-    <t>Target: [[-2 AP, -2 MP, -2 Range, -100% Light resistance]] (00 turns)</t>
-  </si>
-  <si>
-    <t>Caster: [[Reduce max HP by 10%]] (00 turns)</t>
-  </si>
-  <si>
-    <t>Target: [[HP set to 60% of max HP]]</t>
-  </si>
-  <si>
     <t xml:space="preserve">[[Area of effect: - Straight line of cells ]] (Modular area) </t>
   </si>
   <si>
@@ -191,12 +149,6 @@
     <t>[[Area of effect: - Single cell ]]</t>
   </si>
   <si>
-    <t>[[Damage:  15-20 earth ]]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inflicts Earth-type damage on entity.                                                 OR                                                                                                    Summons an unmovable Tomb Stone on an empty cell.                     </t>
-  </si>
-  <si>
     <t>[[Area of effect: - Cross of 1 cell]]</t>
   </si>
   <si>
@@ -206,18 +158,6 @@
     <t>[[Number of turns between two casts: 4 ]]</t>
   </si>
   <si>
-    <t>[[Boost damage dealt by 50%]] (1 turn)</t>
-  </si>
-  <si>
-    <t>[[Return 25% of damage dealt in Dark-type damage ]] (1 turn)</t>
-  </si>
-  <si>
-    <t>Effect name: ''Power''.</t>
-  </si>
-  <si>
-    <t>Effect name: ''Self Consumption''.</t>
-  </si>
-  <si>
     <t>Boost the power of the caster and the entities around him.               The damage dealt are greater, but part of those damage are also taken by the holders of that aura.</t>
   </si>
   <si>
@@ -239,12 +179,6 @@
     <t>Living Ground</t>
   </si>
   <si>
-    <t>Glyph (2 turns)</t>
-  </si>
-  <si>
-    <t>[[Damage:  40 earth ]]</t>
-  </si>
-  <si>
     <t>[[Number of turns between two casts: 3 ]]</t>
   </si>
   <si>
@@ -254,62 +188,371 @@
     <t>[[Range: 0-2 ]]</t>
   </si>
   <si>
-    <t>[[Reduce MP by 2]] (1 turn)</t>
-  </si>
-  <si>
-    <t>Inflicts Earth-type damage.                                                              The glyph dealt damage and slow down when an entity start his turn on it.</t>
-  </si>
-  <si>
-    <t>Effect name: ''Slowness''.</t>
-  </si>
-  <si>
     <t>Soul Reaping</t>
   </si>
   <si>
-    <t>Effect name: ''Blinded''.</t>
-  </si>
-  <si>
-    <t>Effect name: ''Invulnerable''.</t>
-  </si>
-  <si>
-    <t>Effect name: ''Heavy''.</t>
-  </si>
-  <si>
     <t>[[AP: 7 ]]</t>
   </si>
   <si>
     <t>[[Range: 1 ]]</t>
   </si>
   <si>
-    <t>[[Damage:  120 Dark ]]</t>
-  </si>
-  <si>
-    <t>If the target is set K/O: [[Caster +7AP]]</t>
-  </si>
-  <si>
-    <t>If the target is set K/O: [[Target disintegrated]]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inflicts Dark-type damage.                                                                    If the damage kill the target, the caster regain the AP used and the target is desintegrated. </t>
-  </si>
-  <si>
     <t>On enemy: [[Damage:  35-40 dark steal]]</t>
   </si>
   <si>
     <t>On allie:     [[Damage:  75-80 dark steal]]</t>
   </si>
   <si>
-    <t>The caster become invulnerable and unmovable.                               End the turn.</t>
-  </si>
-  <si>
-    <t>Summons a ''Tomb Stone'' [[20% summoner HP, 0 AP, 0 MP, 20% earth resistence, 15% fire resistence, -30% water resistence, 10% air resistence, -50% light resistence, 50% dark resistence]]</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Invulnerable]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (1 turn)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Binding]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (1 turn)</t>
+    </r>
+  </si>
+  <si>
+    <t>The caster become invulnerable and heavy.                                     End the turn.</t>
+  </si>
+  <si>
+    <t>Every entity except the caster loose all they range.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Blindness]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> + 100 levels (2 turns)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[[Reanimated]] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(00 turns) </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[[Zombification]] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>(00 turns)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Blindness]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +2 levels (00 turns)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[[Laziness]] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>+2 levels (00 turns)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[[Slowness]] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>+2 levels (00 turns)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Phobia of Light]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +100 levels (00 turns)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Caster: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Void]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +10 levels (00 turns)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">inflicts Ground-type damage on entity.                                                 OR                                                                                                    Summons an heavy Tomb Stone on an empty cell.                     </t>
+  </si>
+  <si>
+    <t>Summons a ''Tomb Stone'' [[20% summoner HP, 0 AP, 0 MP,         20% ground resistence, 15% fire resistence, -30% water resistence, 10% wind resistence, -50% light resistence, 50% dark resistence]]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tomb Stone: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[[Binding]] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(00 turns) </t>
+    </r>
+  </si>
+  <si>
+    <t>On enemy: [[Damage: 15-20 earth ]]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Over Power]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +50 levels (1 turn)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Self Consumption]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +25 levels (1 turn)</t>
+    </r>
+  </si>
+  <si>
+    <t>Inflicts Ground-type damage.                                                              The glyph dealt damage and slow down when an entity start his turn on it.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [[Damage: 40 ground ]]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">    [[Slowness]] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>+2 levels (1 turn)</t>
+    </r>
+  </si>
+  <si>
+    <t>'Living Ground'' (Passive Glyph) (2 turns)</t>
+  </si>
+  <si>
+    <t>[[Damage: 120 Dark ]]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    Caster: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Stimulated]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +7 levels (1 turn)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">    Permanently K/O.</t>
+  </si>
+  <si>
+    <t>If is set K/O:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inflicts Dark-type damage.                                                                    If the damage kill the target, the caster regain the AP used and the target permanently K/O. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -341,6 +584,12 @@
       <name val="Algerian"/>
       <family val="5"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -368,7 +617,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -400,11 +649,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -418,7 +693,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -435,10 +709,16 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -753,10 +1033,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D28"/>
+  <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,8 +1055,8 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>4</v>
+      <c r="C3" s="7" t="s">
+        <v>1</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -787,8 +1067,8 @@
     </row>
     <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="13" t="s">
-        <v>88</v>
+      <c r="C5" s="12" t="s">
+        <v>58</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -800,21 +1080,21 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -826,7 +1106,7 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D11" s="1"/>
     </row>
@@ -838,96 +1118,80 @@
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="C17" s="9" t="s">
+        <v>56</v>
+      </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="10" t="s">
-        <v>12</v>
+      <c r="C18" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="10" t="s">
-        <v>13</v>
+      <c r="C19" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="10" t="s">
-        <v>14</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="5" t="s">
+        <v>0</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+      <c r="C25" s="8"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
-      <c r="C26" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B27" s="1"/>
-      <c r="C27" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="6"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -937,10 +1201,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D25"/>
+  <dimension ref="B2:D26"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,8 +1223,8 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>76</v>
+      <c r="C3" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -971,8 +1235,8 @@
     </row>
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="13" t="s">
-        <v>85</v>
+      <c r="C5" s="12" t="s">
+        <v>82</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -984,14 +1248,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1003,7 +1267,7 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -1015,7 +1279,7 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -1027,7 +1291,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1038,57 +1302,64 @@
     </row>
     <row r="16" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B16" s="1"/>
-      <c r="C16" s="10" t="s">
-        <v>82</v>
+      <c r="C16" s="9" t="s">
+        <v>78</v>
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="10" t="s">
-        <v>83</v>
+      <c r="C17" s="15" t="s">
+        <v>81</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="15" t="s">
-        <v>84</v>
+      <c r="C18" s="13" t="s">
+        <v>80</v>
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="C19" s="13" t="s">
+        <v>79</v>
+      </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="5" t="s">
+        <v>0</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="9"/>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="6"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1120,8 +1391,8 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>15</v>
+      <c r="C3" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1133,7 +1404,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1145,21 +1416,21 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -1171,7 +1442,7 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D11" s="1"/>
     </row>
@@ -1183,7 +1454,7 @@
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -1195,7 +1466,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="3" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -1207,7 +1478,7 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -1225,7 +1496,7 @@
     <row r="21" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
       <c r="C21" s="5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -1236,9 +1507,7 @@
     </row>
     <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
-      <c r="C23" s="9" t="s">
-        <v>77</v>
-      </c>
+      <c r="C23" s="8"/>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
@@ -1256,8 +1525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1276,8 +1545,8 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>22</v>
+      <c r="C3" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1288,8 +1557,8 @@
     </row>
     <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="11" t="s">
-        <v>23</v>
+      <c r="C5" s="10" t="s">
+        <v>15</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1301,14 +1570,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1320,21 +1589,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -1346,14 +1615,14 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -1365,7 +1634,7 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -1376,15 +1645,15 @@
     </row>
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="10" t="s">
-        <v>86</v>
+      <c r="C19" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
-      <c r="C20" s="10" t="s">
-        <v>87</v>
+      <c r="C20" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -1402,7 +1671,7 @@
     <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
       <c r="C24" s="5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D24" s="1"/>
     </row>
@@ -1413,7 +1682,7 @@
     </row>
     <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
-      <c r="C26" s="9"/>
+      <c r="C26" s="8"/>
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
@@ -1429,10 +1698,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D30"/>
+  <dimension ref="B2:D32"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1451,8 +1720,8 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>32</v>
+      <c r="C3" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1463,8 +1732,8 @@
     </row>
     <row r="5" spans="2:4" ht="97.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="13" t="s">
-        <v>39</v>
+      <c r="C5" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1476,21 +1745,21 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -1502,21 +1771,21 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -1528,7 +1797,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -1540,84 +1809,96 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="10" t="s">
-        <v>38</v>
+      <c r="C19" s="13" t="s">
+        <v>61</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
-      <c r="C20" s="10" t="s">
-        <v>40</v>
+      <c r="C20" s="14" t="s">
+        <v>62</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
-      <c r="C21" s="10" t="s">
-        <v>42</v>
+      <c r="C21" s="13" t="s">
+        <v>64</v>
       </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
-      <c r="C22" s="10" t="s">
-        <v>41</v>
+      <c r="C22" s="13" t="s">
+        <v>65</v>
       </c>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="13" t="s">
+        <v>63</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B24" s="1"/>
+      <c r="C24" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+      <c r="C25" s="9" t="s">
+        <v>67</v>
+      </c>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
-      <c r="C26" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
-      <c r="C28" s="12" t="s">
-        <v>36</v>
-      </c>
+      <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B29" s="1"/>
-      <c r="C29" s="12" t="s">
-        <v>37</v>
+      <c r="C29" s="5" t="s">
+        <v>0</v>
       </c>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="6"/>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B31" s="1"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1630,7 +1911,7 @@
   <dimension ref="B2:D25"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1649,8 +1930,8 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>63</v>
+      <c r="C3" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1661,8 +1942,8 @@
     </row>
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="13" t="s">
-        <v>44</v>
+      <c r="C5" s="12" t="s">
+        <v>30</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1674,14 +1955,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1693,21 +1974,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -1719,7 +2000,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1731,7 +2012,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -1743,7 +2024,7 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="3" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -1761,7 +2042,7 @@
     <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
       <c r="C22" s="5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -1772,7 +2053,7 @@
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
-      <c r="C24" s="9"/>
+      <c r="C24" s="8"/>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
@@ -1788,10 +2069,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D26"/>
+  <dimension ref="B2:D27"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1810,8 +2091,8 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>48</v>
+      <c r="C3" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1822,8 +2103,8 @@
     </row>
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="13" t="s">
-        <v>53</v>
+      <c r="C5" s="12" t="s">
+        <v>68</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1835,14 +2116,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1854,21 +2135,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -1880,7 +2161,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1892,7 +2173,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -1903,50 +2184,57 @@
     </row>
     <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="10" t="s">
-        <v>52</v>
+      <c r="C18" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="59.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:4" ht="78" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
-      <c r="C19" s="14" t="s">
-        <v>89</v>
+      <c r="C19" s="17" t="s">
+        <v>69</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="C20" s="16" t="s">
+        <v>70</v>
+      </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
-      <c r="C23" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
+      <c r="C24" s="5" t="s">
+        <v>0</v>
+      </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" s="9"/>
+      <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="6"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1956,10 +2244,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D29"/>
+  <dimension ref="B2:D24"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1978,8 +2266,8 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>55</v>
+      <c r="C3" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1990,8 +2278,8 @@
     </row>
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="13" t="s">
-        <v>61</v>
+      <c r="C5" s="12" t="s">
+        <v>41</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2003,14 +2291,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -2022,7 +2310,7 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -2034,64 +2322,56 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="C13" s="3"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
-      <c r="C15" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>1</v>
+      <c r="C16" s="9" t="s">
+        <v>72</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="3"/>
+      <c r="C17" s="13" t="s">
+        <v>73</v>
+      </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="3" t="s">
-        <v>54</v>
-      </c>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="10" t="s">
-        <v>58</v>
+      <c r="C21" s="5" t="s">
+        <v>0</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -2100,42 +2380,15 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B23" s="1"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="1"/>
+    </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B25" s="1"/>
-      <c r="C25" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B27" s="1"/>
-      <c r="C27" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B28" s="1"/>
-      <c r="C28" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="6"/>
+      <c r="D24" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2148,7 +2401,7 @@
   <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2167,8 +2420,8 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>62</v>
+      <c r="C3" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2180,7 +2433,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2192,21 +2445,21 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -2218,21 +2471,21 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -2244,7 +2497,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="3" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -2256,7 +2509,7 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -2268,7 +2521,7 @@
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="3" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -2286,7 +2539,7 @@
     <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
       <c r="C23" s="5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D23" s="1"/>
     </row>
@@ -2297,7 +2550,7 @@
     </row>
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="9"/>
+      <c r="C25" s="8"/>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
@@ -2316,7 +2569,7 @@
   <dimension ref="B2:D28"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2335,8 +2588,8 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>67</v>
+      <c r="C3" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2347,7 +2600,7 @@
     </row>
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>74</v>
       </c>
       <c r="D5" s="1"/>
@@ -2360,21 +2613,21 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -2386,21 +2639,21 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -2412,7 +2665,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="3" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -2424,7 +2677,7 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -2435,22 +2688,22 @@
     </row>
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="10" t="s">
-        <v>69</v>
+      <c r="C19" s="18" t="s">
+        <v>77</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
-      <c r="C20" s="10" t="s">
-        <v>73</v>
+      <c r="C20" s="9" t="s">
+        <v>75</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="10" t="s">
-        <v>68</v>
+      <c r="C21" s="9" t="s">
+        <v>76</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -2468,7 +2721,7 @@
     <row r="25" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
       <c r="C25" s="5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -2479,9 +2732,7 @@
     </row>
     <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B27" s="1"/>
-      <c r="C27" s="9" t="s">
-        <v>75</v>
-      </c>
+      <c r="C27" s="8"/>
       <c r="D27" s="1"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Worked on effects doc. + Cleaned half of Druid skills doc.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/_Done/6-GrimReaper/Documentation/GrimReaperSkills.xlsx
+++ b/GameDesign/Class/_Done/6-GrimReaper/Documentation/GrimReaperSkills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="4" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="1-ProtectiveWings" sheetId="1" r:id="rId1"/>
@@ -1203,7 +1203,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -1700,8 +1700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D32"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C24" sqref="C21:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>